<commit_message>
Added SparkFun GP-735T GPS specs
</commit_message>
<xml_diff>
--- a/pad30/Batt.xlsx
+++ b/pad30/Batt.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Vcc</t>
   </si>
   <si>
     <t>ADC2</t>
+  </si>
+  <si>
+    <t>ADC3</t>
+  </si>
+  <si>
+    <t>Vcc(-)</t>
   </si>
 </sst>
 </file>
@@ -57,8 +63,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -135,45 +144,45 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>970</c:v>
+                  <c:v>1022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>910</c:v>
+                  <c:v>959</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>848</c:v>
+                  <c:v>894</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>789</c:v>
+                  <c:v>834</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>733</c:v>
+                  <c:v>771</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>671</c:v>
+                  <c:v>708</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57980032"/>
-        <c:axId val="57981568"/>
+        <c:axId val="56846592"/>
+        <c:axId val="59359232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57980032"/>
+        <c:axId val="56846592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57981568"/>
+        <c:crossAx val="59359232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57981568"/>
+        <c:axId val="59359232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -181,7 +190,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57980032"/>
+        <c:crossAx val="56846592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -194,26 +203,158 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ADC3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>953</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>891</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>767</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="55495296"/>
+        <c:axId val="55493760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="55495296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55493760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="55493760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="55495296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -227,6 +368,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -520,68 +691,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:L13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>16</v>
       </c>
       <c r="B2">
-        <v>970</v>
+        <v>1022</v>
+      </c>
+      <c r="D2">
+        <v>-16</v>
+      </c>
+      <c r="E2">
+        <v>1018</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>910</v>
+        <v>959</v>
+      </c>
+      <c r="D3">
+        <v>-15</v>
+      </c>
+      <c r="E3">
+        <v>953</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>14</v>
       </c>
       <c r="B4">
-        <v>848</v>
+        <v>894</v>
+      </c>
+      <c r="D4">
+        <v>-14</v>
+      </c>
+      <c r="E4">
+        <v>891</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>13</v>
       </c>
       <c r="B5">
-        <v>789</v>
+        <v>834</v>
+      </c>
+      <c r="D5">
+        <v>-13</v>
+      </c>
+      <c r="E5">
+        <v>833</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>12</v>
       </c>
       <c r="B6">
-        <v>733</v>
+        <v>771</v>
+      </c>
+      <c r="D6">
+        <v>-12</v>
+      </c>
+      <c r="E6">
+        <v>767</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>671</v>
+        <v>708</v>
+      </c>
+      <c r="D7">
+        <v>-11</v>
+      </c>
+      <c r="E7">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <f>(62.686+62.171)/2</f>
+        <v>62.4285</v>
+      </c>
+      <c r="B10">
+        <f>(18.41+22.019)/2</f>
+        <v>20.214500000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>